<commit_message>
Requirement Rule XLS file
</commit_message>
<xml_diff>
--- a/loan-application/src/main/resources/com/redhat/demos/dm/loan/rules/RequirementRules.xlsx
+++ b/loan-application/src/main/resources/com/redhat/demos/dm/loan/rules/RequirementRules.xlsx
@@ -44,10 +44,6 @@
     <t>com.stepsoln.rules</t>
   </si>
   <si>
-    <t>com.stepsoln.rules.domain.requirements.RequirementForm,
-com.stepsoln.rules.domain.CaseData</t>
-  </si>
-  <si>
     <t>$form:RequirementForm</t>
   </si>
   <si>
@@ -138,6 +134,10 @@
   </si>
   <si>
     <t>GA</t>
+  </si>
+  <si>
+    <t>com.redhat.demos.dm.loan.model.RequirementForm,
+com.redhat.demos.dm.loan.model.CaseData</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -726,7 +726,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -757,10 +757,10 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="27"/>
@@ -768,19 +768,19 @@
     <row r="7" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="28" t="s">
         <v>14</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,36 +788,36 @@
         <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>23</v>
       </c>
       <c r="F9" s="29" t="str">
         <f>LOWER(TRUE)</f>
@@ -826,19 +826,19 @@
     </row>
     <row r="10" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>25</v>
-      </c>
       <c r="C10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" t="str">
         <f>LOWER(TRUE)</f>
@@ -847,19 +847,19 @@
     </row>
     <row r="11" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="C11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>33</v>
       </c>
       <c r="F11" t="str">
         <f>LOWER(TRUE)</f>

</xml_diff>